<commit_message>
Update explanation as agreed
</commit_message>
<xml_diff>
--- a/scenarios/cough/processes/Explanation.xlsx
+++ b/scenarios/cough/processes/Explanation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -52,31 +52,68 @@
     <t xml:space="preserve">CODE</t>
   </si>
   <si>
-    <t xml:space="preserve">IF [item] THEN GO(dummy) ELSE (FOR item IN [cart] DO (INJECT_WITH(Explanation, item)), FINISH())</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dummy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dummy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Some question</t>
+    <t xml:space="preserve">IF [item] THEN GO(variables) ELSE (FOR item IN [cart] DO (INJECT_WITH(Explanation, item)), FINISH())</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_api_category = TO_TEXT(SELECT a.CategoryChoice FROM Products p JOIN API a ON p.APIID == a.ID WHERE p.ID == [item]), item_med_form = TO_TEXT(SELECT MedFormID FROM Products WHERE ID == [item]), SAVE(item_api_category), SAVE(item_med_form), GO(product)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{SELECT [item_api_category] FROM Explanation WHERE MedFormID == [item_med_form]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT * FROM Products WHERE ID == [item]</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
   </si>
   <si>
-    <t xml:space="preserve">Some answer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FINISH()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Some other</t>
+    <t xml:space="preserve">Very nice :D</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">DELETE(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">item_api_category), DELETE(item_med_form), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">FINISH()</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -200,7 +237,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -284,13 +321,13 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.39453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="84.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
   </cols>
@@ -340,32 +377,38 @@
         <v>12</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>15</v>
+      </c>
       <c r="C4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="F4" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>